<commit_message>
Adding in notebook version of major python scripts for reserach purposes
</commit_message>
<xml_diff>
--- a/Input & Output/Output/Post Analysis/all_field_data_monthly.xlsx
+++ b/Input & Output/Output/Post Analysis/all_field_data_monthly.xlsx
@@ -11629,10 +11629,10 @@
         <v>42736</v>
       </c>
       <c r="B166" t="n">
-        <v>5946.377688172043</v>
+        <v>5665</v>
       </c>
       <c r="C166" t="n">
-        <v>16271.64516129032</v>
+        <v>14153</v>
       </c>
       <c r="D166" t="n">
         <v>17705.69220430107</v>
@@ -11694,10 +11694,10 @@
         <v>42767</v>
       </c>
       <c r="B167" t="n">
-        <v>5755.407738095239</v>
+        <v>0</v>
       </c>
       <c r="C167" t="n">
-        <v>15788.09077380952</v>
+        <v>0</v>
       </c>
       <c r="D167" t="n">
         <v>16974.92113095238</v>
@@ -11748,7 +11748,7 @@
         <v>0.04365114795918366</v>
       </c>
       <c r="T167" t="n">
-        <v>5946.377688172043</v>
+        <v>5665</v>
       </c>
       <c r="U167" t="n">
         <v>6010000</v>
@@ -11759,10 +11759,10 @@
         <v>42795</v>
       </c>
       <c r="B168" t="n">
-        <v>5770.697580645161</v>
+        <v>0</v>
       </c>
       <c r="C168" t="n">
-        <v>15580.03225806452</v>
+        <v>0</v>
       </c>
       <c r="D168" t="n">
         <v>16574.23790322581</v>
@@ -11813,7 +11813,7 @@
         <v>0.2294719042663891</v>
       </c>
       <c r="T168" t="n">
-        <v>5755.407738095239</v>
+        <v>0</v>
       </c>
       <c r="U168" t="n">
         <v>6010000</v>
@@ -11824,10 +11824,10 @@
         <v>42826</v>
       </c>
       <c r="B169" t="n">
-        <v>5120.201388888889</v>
+        <v>0</v>
       </c>
       <c r="C169" t="n">
-        <v>13597.32222222222</v>
+        <v>0</v>
       </c>
       <c r="D169" t="n">
         <v>15249.43472222222</v>
@@ -11878,7 +11878,7 @@
         <v>86.27932844444443</v>
       </c>
       <c r="T169" t="n">
-        <v>5770.697580645161</v>
+        <v>0</v>
       </c>
       <c r="U169" t="n">
         <v>6010000</v>
@@ -11889,10 +11889,10 @@
         <v>42856</v>
       </c>
       <c r="B170" t="n">
-        <v>5182.504032258064</v>
+        <v>0</v>
       </c>
       <c r="C170" t="n">
-        <v>13646.29166666667</v>
+        <v>0</v>
       </c>
       <c r="D170" t="n">
         <v>15093.7123655914</v>
@@ -11943,7 +11943,7 @@
         <v>158.7112295525494</v>
       </c>
       <c r="T170" t="n">
-        <v>5120.201388888889</v>
+        <v>0</v>
       </c>
       <c r="U170" t="n">
         <v>6010000</v>
@@ -11954,10 +11954,10 @@
         <v>42887</v>
       </c>
       <c r="B171" t="n">
-        <v>5679.984722222222</v>
+        <v>0</v>
       </c>
       <c r="C171" t="n">
-        <v>14799.18888888889</v>
+        <v>0</v>
       </c>
       <c r="D171" t="n">
         <v>16253.53611111111</v>
@@ -12008,7 +12008,7 @@
         <v>375.7782250000001</v>
       </c>
       <c r="T171" t="n">
-        <v>5182.504032258064</v>
+        <v>0</v>
       </c>
       <c r="U171" t="n">
         <v>6010000</v>
@@ -12019,10 +12019,10 @@
         <v>42917</v>
       </c>
       <c r="B172" t="n">
-        <v>5951.712365591397</v>
+        <v>0</v>
       </c>
       <c r="C172" t="n">
-        <v>15572.87365591398</v>
+        <v>0</v>
       </c>
       <c r="D172" t="n">
         <v>16618.16666666667</v>
@@ -12073,7 +12073,7 @@
         <v>468.8761577523411</v>
       </c>
       <c r="T172" t="n">
-        <v>5679.984722222222</v>
+        <v>0</v>
       </c>
       <c r="U172" t="n">
         <v>6010000</v>
@@ -12084,10 +12084,10 @@
         <v>42948</v>
       </c>
       <c r="B173" t="n">
-        <v>5852.674731182796</v>
+        <v>0</v>
       </c>
       <c r="C173" t="n">
-        <v>15259.55510752688</v>
+        <v>0</v>
       </c>
       <c r="D173" t="n">
         <v>16199.52553763441</v>
@@ -12138,7 +12138,7 @@
         <v>408.5614568158168</v>
       </c>
       <c r="T173" t="n">
-        <v>5951.712365591397</v>
+        <v>0</v>
       </c>
       <c r="U173" t="n">
         <v>6010000</v>
@@ -12149,10 +12149,10 @@
         <v>42979</v>
       </c>
       <c r="B174" t="n">
-        <v>5727.665277777778</v>
+        <v>0</v>
       </c>
       <c r="C174" t="n">
-        <v>14833.28888888889</v>
+        <v>0</v>
       </c>
       <c r="D174" t="n">
         <v>15531.93194444444</v>
@@ -12203,7 +12203,7 @@
         <v>349.5778089999999</v>
       </c>
       <c r="T174" t="n">
-        <v>5852.674731182796</v>
+        <v>0</v>
       </c>
       <c r="U174" t="n">
         <v>6010000</v>
@@ -12214,10 +12214,10 @@
         <v>43009</v>
       </c>
       <c r="B175" t="n">
-        <v>5207.611559139785</v>
+        <v>0</v>
       </c>
       <c r="C175" t="n">
-        <v>13894.97983870968</v>
+        <v>0</v>
       </c>
       <c r="D175" t="n">
         <v>15174.46639784946</v>
@@ -12268,7 +12268,7 @@
         <v>179.4562730489073</v>
       </c>
       <c r="T175" t="n">
-        <v>5727.665277777778</v>
+        <v>0</v>
       </c>
       <c r="U175" t="n">
         <v>6010000</v>
@@ -12279,10 +12279,10 @@
         <v>43040</v>
       </c>
       <c r="B176" t="n">
-        <v>5524.329166666666</v>
+        <v>0</v>
       </c>
       <c r="C176" t="n">
-        <v>15214.7375</v>
+        <v>0</v>
       </c>
       <c r="D176" t="n">
         <v>16526.81527777778</v>
@@ -12333,7 +12333,7 @@
         <v>16.09881877777778</v>
       </c>
       <c r="T176" t="n">
-        <v>5207.611559139785</v>
+        <v>0</v>
       </c>
       <c r="U176" t="n">
         <v>6010000</v>
@@ -12344,10 +12344,10 @@
         <v>43070</v>
       </c>
       <c r="B177" t="n">
-        <v>5692.653225806452</v>
+        <v>0</v>
       </c>
       <c r="C177" t="n">
-        <v>16493.22311827957</v>
+        <v>0</v>
       </c>
       <c r="D177" t="n">
         <v>18063.3938172043</v>
@@ -12398,7 +12398,7 @@
         <v>23.06478085327783</v>
       </c>
       <c r="T177" t="n">
-        <v>5524.329166666666</v>
+        <v>0</v>
       </c>
       <c r="U177" t="n">
         <v>6010000</v>
@@ -12409,10 +12409,10 @@
         <v>43101</v>
       </c>
       <c r="B178" t="n">
-        <v>5916.83870967742</v>
+        <v>5917.42799461642</v>
       </c>
       <c r="C178" t="n">
-        <v>17072.60887096774</v>
+        <v>17072.91924629879</v>
       </c>
       <c r="D178" t="n">
         <v>18766.59811827957</v>
@@ -12463,7 +12463,7 @@
         <v>28.21323163371488</v>
       </c>
       <c r="T178" t="n">
-        <v>5692.653225806452</v>
+        <v>0</v>
       </c>
       <c r="U178" t="n">
         <v>6082000</v>
@@ -12528,7 +12528,7 @@
         <v>2.411365306122449</v>
       </c>
       <c r="T179" t="n">
-        <v>5916.83870967742</v>
+        <v>5917.42799461642</v>
       </c>
       <c r="U179" t="n">
         <v>6082000</v>

</xml_diff>

<commit_message>
fixing minors bugs in demand and supply dataset generation
</commit_message>
<xml_diff>
--- a/Input & Output/Output/Post Analysis/all_field_data_monthly.xlsx
+++ b/Input & Output/Output/Post Analysis/all_field_data_monthly.xlsx
@@ -8515,7 +8515,7 @@
         <v>17322.02822580645</v>
       </c>
       <c r="D118" t="n">
-        <v>23.0255376344086</v>
+        <v>19091.93279569893</v>
       </c>
       <c r="E118" t="n">
         <v>32.50404569892473</v>
@@ -8580,7 +8580,7 @@
         <v>17475.22470238095</v>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>18825.34523809524</v>
       </c>
       <c r="E119" t="n">
         <v>29.32602678571429</v>
@@ -8645,7 +8645,7 @@
         <v>16077.18413978495</v>
       </c>
       <c r="D120" t="n">
-        <v>0</v>
+        <v>17232.53897849462</v>
       </c>
       <c r="E120" t="n">
         <v>29.7092876344086</v>
@@ -8710,7 +8710,7 @@
         <v>15201.54722222222</v>
       </c>
       <c r="D121" t="n">
-        <v>0</v>
+        <v>16683.79444444444</v>
       </c>
       <c r="E121" t="n">
         <v>27.27879166666667</v>
@@ -8775,7 +8775,7 @@
         <v>14494.07123655914</v>
       </c>
       <c r="D122" t="n">
-        <v>0</v>
+        <v>16196.16532258064</v>
       </c>
       <c r="E122" t="n">
         <v>25.05255376344086</v>
@@ -8840,7 +8840,7 @@
         <v>15522.30555555555</v>
       </c>
       <c r="D123" t="n">
-        <v>0</v>
+        <v>16970.33611111111</v>
       </c>
       <c r="E123" t="n">
         <v>27.49077777777778</v>
@@ -8905,7 +8905,7 @@
         <v>17098.99462365592</v>
       </c>
       <c r="D124" t="n">
-        <v>0</v>
+        <v>18394.55376344086</v>
       </c>
       <c r="E124" t="n">
         <v>33.51479838709677</v>
@@ -8970,7 +8970,7 @@
         <v>16263.44086021505</v>
       </c>
       <c r="D125" t="n">
-        <v>0</v>
+        <v>17483.94758064516</v>
       </c>
       <c r="E125" t="n">
         <v>28.31301075268818</v>
@@ -9035,7 +9035,7 @@
         <v>15053.24166666667</v>
       </c>
       <c r="D126" t="n">
-        <v>0</v>
+        <v>16126.75833333333</v>
       </c>
       <c r="E126" t="n">
         <v>20.75879166666667</v>
@@ -9100,7 +9100,7 @@
         <v>14967.72580645161</v>
       </c>
       <c r="D127" t="n">
-        <v>0</v>
+        <v>16221.31182795699</v>
       </c>
       <c r="E127" t="n">
         <v>23.42118279569893</v>
@@ -9165,7 +9165,7 @@
         <v>16164.99166666667</v>
       </c>
       <c r="D128" t="n">
-        <v>0</v>
+        <v>17593.7875</v>
       </c>
       <c r="E128" t="n">
         <v>14.81556944444444</v>
@@ -9230,7 +9230,7 @@
         <v>17209.17338709677</v>
       </c>
       <c r="D129" t="n">
-        <v>0</v>
+        <v>18630.69758064516</v>
       </c>
       <c r="E129" t="n">
         <v>27.91994623655914</v>
@@ -9295,7 +9295,7 @@
         <v>18297.59811827957</v>
       </c>
       <c r="D130" t="n">
-        <v>0</v>
+        <v>19906.20564516129</v>
       </c>
       <c r="E130" t="n">
         <v>52.95629032258065</v>
@@ -9360,7 +9360,7 @@
         <v>17955.70089285714</v>
       </c>
       <c r="D131" t="n">
-        <v>0</v>
+        <v>17990.8556547619</v>
       </c>
       <c r="E131" t="n">
         <v>60.76348214285714</v>
@@ -9425,7 +9425,7 @@
         <v>17037.32392473118</v>
       </c>
       <c r="D132" t="n">
-        <v>0</v>
+        <v>17432.80107526882</v>
       </c>
       <c r="E132" t="n">
         <v>75.01715053763441</v>
@@ -9490,7 +9490,7 @@
         <v>15051.13055555556</v>
       </c>
       <c r="D133" t="n">
-        <v>0</v>
+        <v>16188.03888888889</v>
       </c>
       <c r="E133" t="n">
         <v>33.80997222222222</v>
@@ -9555,7 +9555,7 @@
         <v>14306.88172043011</v>
       </c>
       <c r="D134" t="n">
-        <v>0</v>
+        <v>16319.80241935484</v>
       </c>
       <c r="E134" t="n">
         <v>17.9589247311828</v>
@@ -9620,7 +9620,7 @@
         <v>15589.05833333333</v>
       </c>
       <c r="D135" t="n">
-        <v>0</v>
+        <v>17168.31527777778</v>
       </c>
       <c r="E135" t="n">
         <v>27.337625</v>
@@ -9685,7 +9685,7 @@
         <v>15752.64919354839</v>
       </c>
       <c r="D136" t="n">
-        <v>0</v>
+        <v>17132.45295698925</v>
       </c>
       <c r="E136" t="n">
         <v>23.99661290322581</v>
@@ -9750,7 +9750,7 @@
         <v>15750.0376344086</v>
       </c>
       <c r="D137" t="n">
-        <v>0</v>
+        <v>17084.39919354839</v>
       </c>
       <c r="E137" t="n">
         <v>22.82049731182796</v>
@@ -9815,7 +9815,7 @@
         <v>15052.34861111111</v>
       </c>
       <c r="D138" t="n">
-        <v>0</v>
+        <v>17149.18472222222</v>
       </c>
       <c r="E138" t="n">
         <v>13.92965277777778</v>
@@ -9880,7 +9880,7 @@
         <v>14542.74059139785</v>
       </c>
       <c r="D139" t="n">
-        <v>0</v>
+        <v>16431.7997311828</v>
       </c>
       <c r="E139" t="n">
         <v>11.78736559139785</v>
@@ -9945,7 +9945,7 @@
         <v>15953.81666666667</v>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>18045.04166666667</v>
       </c>
       <c r="E140" t="n">
         <v>11.00595833333333</v>
@@ -10010,7 +10010,7 @@
         <v>16346.55241935484</v>
       </c>
       <c r="D141" t="n">
-        <v>0</v>
+        <v>18366.11827956989</v>
       </c>
       <c r="E141" t="n">
         <v>14.78576612903226</v>
@@ -10075,7 +10075,7 @@
         <v>17633.32930107527</v>
       </c>
       <c r="D142" t="n">
-        <v>19881.40994623656</v>
+        <v>19906.20967741936</v>
       </c>
       <c r="E142" t="n">
         <v>30.00384408602151</v>
@@ -11629,10 +11629,10 @@
         <v>42736</v>
       </c>
       <c r="B166" t="n">
-        <v>5665</v>
+        <v>5946.377688172043</v>
       </c>
       <c r="C166" t="n">
-        <v>14153</v>
+        <v>16271.64516129032</v>
       </c>
       <c r="D166" t="n">
         <v>17705.69220430107</v>
@@ -11694,10 +11694,10 @@
         <v>42767</v>
       </c>
       <c r="B167" t="n">
-        <v>0</v>
+        <v>5755.407738095239</v>
       </c>
       <c r="C167" t="n">
-        <v>0</v>
+        <v>15788.09077380952</v>
       </c>
       <c r="D167" t="n">
         <v>16974.92113095238</v>
@@ -11748,7 +11748,7 @@
         <v>0.04365114795918366</v>
       </c>
       <c r="T167" t="n">
-        <v>5665</v>
+        <v>5946.377688172043</v>
       </c>
       <c r="U167" t="n">
         <v>6010000</v>
@@ -11759,10 +11759,10 @@
         <v>42795</v>
       </c>
       <c r="B168" t="n">
-        <v>0</v>
+        <v>5770.697580645161</v>
       </c>
       <c r="C168" t="n">
-        <v>0</v>
+        <v>15580.03225806452</v>
       </c>
       <c r="D168" t="n">
         <v>16574.23790322581</v>
@@ -11813,7 +11813,7 @@
         <v>0.2294719042663891</v>
       </c>
       <c r="T168" t="n">
-        <v>0</v>
+        <v>5755.407738095239</v>
       </c>
       <c r="U168" t="n">
         <v>6010000</v>
@@ -11824,10 +11824,10 @@
         <v>42826</v>
       </c>
       <c r="B169" t="n">
-        <v>0</v>
+        <v>5120.201388888889</v>
       </c>
       <c r="C169" t="n">
-        <v>0</v>
+        <v>13597.32222222222</v>
       </c>
       <c r="D169" t="n">
         <v>15249.43472222222</v>
@@ -11878,7 +11878,7 @@
         <v>86.27932844444443</v>
       </c>
       <c r="T169" t="n">
-        <v>0</v>
+        <v>5770.697580645161</v>
       </c>
       <c r="U169" t="n">
         <v>6010000</v>
@@ -11889,10 +11889,10 @@
         <v>42856</v>
       </c>
       <c r="B170" t="n">
-        <v>0</v>
+        <v>5182.504032258064</v>
       </c>
       <c r="C170" t="n">
-        <v>0</v>
+        <v>13646.29166666667</v>
       </c>
       <c r="D170" t="n">
         <v>15093.7123655914</v>
@@ -11943,7 +11943,7 @@
         <v>158.7112295525494</v>
       </c>
       <c r="T170" t="n">
-        <v>0</v>
+        <v>5120.201388888889</v>
       </c>
       <c r="U170" t="n">
         <v>6010000</v>
@@ -11954,10 +11954,10 @@
         <v>42887</v>
       </c>
       <c r="B171" t="n">
-        <v>0</v>
+        <v>5679.984722222222</v>
       </c>
       <c r="C171" t="n">
-        <v>0</v>
+        <v>14799.18888888889</v>
       </c>
       <c r="D171" t="n">
         <v>16253.53611111111</v>
@@ -12008,7 +12008,7 @@
         <v>375.7782250000001</v>
       </c>
       <c r="T171" t="n">
-        <v>0</v>
+        <v>5182.504032258064</v>
       </c>
       <c r="U171" t="n">
         <v>6010000</v>
@@ -12019,10 +12019,10 @@
         <v>42917</v>
       </c>
       <c r="B172" t="n">
-        <v>0</v>
+        <v>5951.712365591397</v>
       </c>
       <c r="C172" t="n">
-        <v>0</v>
+        <v>15572.87365591398</v>
       </c>
       <c r="D172" t="n">
         <v>16618.16666666667</v>
@@ -12073,7 +12073,7 @@
         <v>468.8761577523411</v>
       </c>
       <c r="T172" t="n">
-        <v>0</v>
+        <v>5679.984722222222</v>
       </c>
       <c r="U172" t="n">
         <v>6010000</v>
@@ -12084,10 +12084,10 @@
         <v>42948</v>
       </c>
       <c r="B173" t="n">
-        <v>0</v>
+        <v>5852.674731182796</v>
       </c>
       <c r="C173" t="n">
-        <v>0</v>
+        <v>15259.55510752688</v>
       </c>
       <c r="D173" t="n">
         <v>16199.52553763441</v>
@@ -12138,7 +12138,7 @@
         <v>408.5614568158168</v>
       </c>
       <c r="T173" t="n">
-        <v>0</v>
+        <v>5951.712365591397</v>
       </c>
       <c r="U173" t="n">
         <v>6010000</v>
@@ -12149,10 +12149,10 @@
         <v>42979</v>
       </c>
       <c r="B174" t="n">
-        <v>0</v>
+        <v>5727.665277777778</v>
       </c>
       <c r="C174" t="n">
-        <v>0</v>
+        <v>14833.28888888889</v>
       </c>
       <c r="D174" t="n">
         <v>15531.93194444444</v>
@@ -12203,7 +12203,7 @@
         <v>349.5778089999999</v>
       </c>
       <c r="T174" t="n">
-        <v>0</v>
+        <v>5852.674731182796</v>
       </c>
       <c r="U174" t="n">
         <v>6010000</v>
@@ -12214,10 +12214,10 @@
         <v>43009</v>
       </c>
       <c r="B175" t="n">
-        <v>0</v>
+        <v>5207.611559139785</v>
       </c>
       <c r="C175" t="n">
-        <v>0</v>
+        <v>13894.97983870968</v>
       </c>
       <c r="D175" t="n">
         <v>15174.46639784946</v>
@@ -12268,7 +12268,7 @@
         <v>179.4562730489073</v>
       </c>
       <c r="T175" t="n">
-        <v>0</v>
+        <v>5727.665277777778</v>
       </c>
       <c r="U175" t="n">
         <v>6010000</v>
@@ -12279,10 +12279,10 @@
         <v>43040</v>
       </c>
       <c r="B176" t="n">
-        <v>0</v>
+        <v>5524.329166666666</v>
       </c>
       <c r="C176" t="n">
-        <v>0</v>
+        <v>15214.7375</v>
       </c>
       <c r="D176" t="n">
         <v>16526.81527777778</v>
@@ -12333,7 +12333,7 @@
         <v>16.09881877777778</v>
       </c>
       <c r="T176" t="n">
-        <v>0</v>
+        <v>5207.611559139785</v>
       </c>
       <c r="U176" t="n">
         <v>6010000</v>
@@ -12344,10 +12344,10 @@
         <v>43070</v>
       </c>
       <c r="B177" t="n">
-        <v>0</v>
+        <v>5692.653225806452</v>
       </c>
       <c r="C177" t="n">
-        <v>0</v>
+        <v>16493.22311827957</v>
       </c>
       <c r="D177" t="n">
         <v>18063.3938172043</v>
@@ -12398,7 +12398,7 @@
         <v>23.06478085327783</v>
       </c>
       <c r="T177" t="n">
-        <v>0</v>
+        <v>5524.329166666666</v>
       </c>
       <c r="U177" t="n">
         <v>6010000</v>
@@ -12409,10 +12409,10 @@
         <v>43101</v>
       </c>
       <c r="B178" t="n">
-        <v>5917.42799461642</v>
+        <v>5916.83870967742</v>
       </c>
       <c r="C178" t="n">
-        <v>17072.91924629879</v>
+        <v>17072.60887096774</v>
       </c>
       <c r="D178" t="n">
         <v>18766.59811827957</v>
@@ -12463,7 +12463,7 @@
         <v>28.21323163371488</v>
       </c>
       <c r="T178" t="n">
-        <v>0</v>
+        <v>5692.653225806452</v>
       </c>
       <c r="U178" t="n">
         <v>6082000</v>
@@ -12528,7 +12528,7 @@
         <v>2.411365306122449</v>
       </c>
       <c r="T179" t="n">
-        <v>5917.42799461642</v>
+        <v>5916.83870967742</v>
       </c>
       <c r="U179" t="n">
         <v>6082000</v>

</xml_diff>